<commit_message>
add modal timeline e modal component
</commit_message>
<xml_diff>
--- a/NotasTimeline.xlsx
+++ b/NotasTimeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reina\Desktop\ProfissaoProgramador\sistema-uranor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProfissaoProgramador\sistema-uranor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9368004B-AFD5-48C6-99E0-A59C6977E58B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B925B5DB-6E62-48F3-AA69-B0CC79EDC8CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{B2553BE9-4389-47AF-9500-BA9C939D5125}"/>
+    <workbookView xWindow="19080" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{B2553BE9-4389-47AF-9500-BA9C939D5125}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
   <si>
     <t>Evento</t>
   </si>
@@ -93,12 +93,6 @@
     <t>Mudança de Templo</t>
   </si>
   <si>
-    <t>Novo Componente</t>
-  </si>
-  <si>
-    <t>Deixou Componente</t>
-  </si>
-  <si>
     <t>Entregou Armas</t>
   </si>
   <si>
@@ -132,18 +126,6 @@
     <t>Transferido de &lt;Antigo&gt; para o templo de &lt;Novo&gt;</t>
   </si>
   <si>
-    <t>Passou a ter &lt;Mestre&gt; como &lt;Pad, Mad ou Esc&gt;</t>
-  </si>
-  <si>
-    <t>Assumiu como &lt;Pad, Mad ou Esc&gt; de &lt;Mestre&gt;</t>
-  </si>
-  <si>
-    <t>Deixou de ser &lt;Pad, Mad ou Esc&gt; de &lt;Mestre&gt;.</t>
-  </si>
-  <si>
-    <t>&lt;Mestre&gt; deixou de ser seu &lt;Pad, Mad ou Esc&gt;.</t>
-  </si>
-  <si>
     <t>Entregou as Armas</t>
   </si>
   <si>
@@ -153,9 +135,6 @@
     <t>OBS: Se for a primeira vez que recebeu mentor, adicionar ministro também</t>
   </si>
   <si>
-    <t>Recebeu cavaleiro/Guia missionária</t>
-  </si>
-  <si>
     <t>Concluiu Curso de 7° Raio</t>
   </si>
   <si>
@@ -234,12 +213,6 @@
     <t>Antigo/Novo</t>
   </si>
   <si>
-    <t>Nome do Mestre</t>
-  </si>
-  <si>
-    <t>Pad, Mad, Esc/Nome Comp</t>
-  </si>
-  <si>
     <t xml:space="preserve"> evento_id: number/Autoincrement</t>
   </si>
   <si>
@@ -255,10 +228,10 @@
     <t>tipo: string</t>
   </si>
   <si>
-    <t>param: string</t>
-  </si>
-  <si>
     <t>PARA BANCO DE DADOS</t>
+  </si>
+  <si>
+    <t>observ: text</t>
   </si>
 </sst>
 </file>
@@ -294,14 +267,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C13951-DB11-4354-A62B-E6A817FBBEEC}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,7 +599,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -640,10 +607,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -654,10 +621,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -668,10 +635,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -682,10 +649,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -696,10 +663,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -710,10 +677,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -724,10 +691,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -738,10 +705,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -752,10 +719,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -766,10 +733,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -783,7 +750,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -794,10 +761,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -808,16 +775,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D14">
         <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -825,16 +792,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D15">
         <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -842,10 +809,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D16">
         <v>5</v>
@@ -856,10 +823,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D17">
         <v>5</v>
@@ -867,13 +834,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D18">
         <v>9</v>
@@ -881,7 +848,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -889,10 +856,10 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D21">
         <v>3</v>
@@ -903,10 +870,10 @@
         <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D22">
         <v>5</v>
@@ -917,10 +884,10 @@
         <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D23">
         <v>5</v>
@@ -928,13 +895,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
         <v>29</v>
       </c>
-      <c r="B24" t="s">
-        <v>31</v>
-      </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D24">
         <v>7</v>
@@ -942,13 +909,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
         <v>30</v>
       </c>
-      <c r="B25" t="s">
-        <v>32</v>
-      </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D25">
         <v>7</v>
@@ -959,10 +926,10 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -973,147 +940,93 @@
         <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" s="2">
-        <v>6</v>
+        <v>50</v>
+      </c>
+      <c r="D28">
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>23</v>
+      <c r="A30" t="s">
+        <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" t="s">
-        <v>70</v>
-      </c>
-      <c r="D31" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="D30">
+        <v>8</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" t="s">
-        <v>57</v>
-      </c>
-      <c r="D32">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" t="s">
-        <v>57</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>27</v>
-      </c>
-      <c r="B34" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" t="s">
-        <v>57</v>
-      </c>
-      <c r="D34">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A30:A31"/>
-  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>